<commit_message>
modify computation and reduce file size
</commit_message>
<xml_diff>
--- a/results/comparaison/GM/azimuth/max_normalized.xlsx
+++ b/results/comparaison/GM/azimuth/max_normalized.xlsx
@@ -810,6 +810,9 @@
       <c r="AS2">
         <v>1</v>
       </c>
+      <c r="AT2">
+        <v>1</v>
+      </c>
       <c r="AU2">
         <v>1</v>
       </c>
@@ -856,9 +859,6 @@
         <v>1</v>
       </c>
       <c r="BJ2">
-        <v>1</v>
-      </c>
-      <c r="BK2">
         <v>1</v>
       </c>
       <c r="BL2">
@@ -980,415 +980,529 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="C3">
+        <v>2.703703703703705</v>
+      </c>
+      <c r="D3">
+        <v>1.890909090909091</v>
+      </c>
+      <c r="E3">
         <v>1.235849056603774</v>
       </c>
-      <c r="C3">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>2.799999999999999</v>
+      </c>
+      <c r="I3">
+        <v>1.416666666666667</v>
+      </c>
+      <c r="J3">
         <v>0.5212765957446808</v>
       </c>
-      <c r="D3">
-        <v>0.9761904761904762</v>
-      </c>
-      <c r="E3">
-        <v>1.492957746478873</v>
-      </c>
-      <c r="F3">
+      <c r="K3">
         <v>1.283582089552239</v>
       </c>
-      <c r="G3">
-        <v>1.705882352941177</v>
-      </c>
-      <c r="H3">
+      <c r="L3">
+        <v>3.159090909090908</v>
+      </c>
+      <c r="M3">
+        <v>1.333333333333333</v>
+      </c>
+      <c r="N3">
         <v>1.321739130434782</v>
       </c>
-      <c r="I3">
+      <c r="O3">
         <v>0.9090909090909091</v>
       </c>
-      <c r="L3">
-        <v>1.309859154929577</v>
-      </c>
-      <c r="N3">
+      <c r="P3">
+        <v>3.081632653061224</v>
+      </c>
+      <c r="Q3">
         <v>0.7407407407407407</v>
       </c>
-      <c r="P3">
-        <v>1.499999999999999</v>
-      </c>
-      <c r="R3">
-        <v>1.46969696969697</v>
-      </c>
-      <c r="S3">
-        <v>1.321100917431193</v>
-      </c>
       <c r="T3">
-        <v>2.566666666666666</v>
+        <v>0.9371069182389938</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3">
-        <v>2.166666666666667</v>
-      </c>
-      <c r="X3">
-        <v>2.799999999999999</v>
+        <v>1.694117647058823</v>
+      </c>
+      <c r="W3">
+        <v>1.060975609756097</v>
       </c>
       <c r="Y3">
-        <v>1.171428571428571</v>
+        <v>1.700000000000001</v>
       </c>
       <c r="Z3">
+        <v>1.328767123287671</v>
+      </c>
+      <c r="AA3">
+        <v>0.07236842105263155</v>
+      </c>
+      <c r="AC3">
+        <v>0.8944099378881988</v>
+      </c>
+      <c r="AD3">
+        <v>0.9909909909909909</v>
+      </c>
+      <c r="AF3">
+        <v>0.9034482758620688</v>
+      </c>
+      <c r="AG3">
+        <v>0.4928571428571429</v>
+      </c>
+      <c r="AI3">
+        <v>1.363636363636364</v>
+      </c>
+      <c r="AJ3">
+        <v>1.326086956521739</v>
+      </c>
+      <c r="AK3">
+        <v>1</v>
+      </c>
+      <c r="AL3">
+        <v>0.944444444444445</v>
+      </c>
+      <c r="AM3">
+        <v>0.9795918367346939</v>
+      </c>
+      <c r="AN3">
+        <v>1.052238805970149</v>
+      </c>
+      <c r="AO3">
+        <v>1.060869565217391</v>
+      </c>
+      <c r="AP3">
+        <v>0.9536423841059603</v>
+      </c>
+      <c r="AQ3">
+        <v>1.633802816901408</v>
+      </c>
+      <c r="AR3">
+        <v>1.794871794871794</v>
+      </c>
+      <c r="AT3">
+        <v>1.169642857142857</v>
+      </c>
+      <c r="AU3">
+        <v>9.75</v>
+      </c>
+      <c r="AV3">
+        <v>1.583333333333333</v>
+      </c>
+      <c r="AW3">
+        <v>0.8870967741935484</v>
+      </c>
+      <c r="AX3">
+        <v>1.823529411764706</v>
+      </c>
+      <c r="AY3">
+        <v>0.7599999999999998</v>
+      </c>
+      <c r="BA3">
+        <v>0.3373493975903615</v>
+      </c>
+      <c r="BB3">
+        <v>1.428571428571429</v>
+      </c>
+      <c r="BC3">
+        <v>0.8405797101449274</v>
+      </c>
+      <c r="BD3">
+        <v>0.71875</v>
+      </c>
+      <c r="BE3">
+        <v>0.650485436893204</v>
+      </c>
+      <c r="BF3">
+        <v>1.852941176470587</v>
+      </c>
+      <c r="BH3">
+        <v>0.4775280898876405</v>
+      </c>
+      <c r="BI3">
+        <v>0.5433070866141733</v>
+      </c>
+      <c r="BJ3">
+        <v>0.3235294117647058</v>
+      </c>
+      <c r="BL3">
+        <v>1.083333333333333</v>
+      </c>
+      <c r="BN3">
+        <v>1.083333333333333</v>
+      </c>
+      <c r="BO3">
+        <v>1.028985507246377</v>
+      </c>
+      <c r="BP3">
+        <v>75.49999999999999</v>
+      </c>
+      <c r="BQ3">
+        <v>0.8630952380952382</v>
+      </c>
+      <c r="BR3">
+        <v>0.9277108433734939</v>
+      </c>
+      <c r="BS3">
+        <v>0.3846153846153846</v>
+      </c>
+      <c r="BT3">
+        <v>1.184615384615384</v>
+      </c>
+      <c r="BU3">
+        <v>1.017751479289941</v>
+      </c>
+      <c r="BV3">
+        <v>1.202702702702703</v>
+      </c>
+      <c r="BW3">
+        <v>0.9874999999999999</v>
+      </c>
+      <c r="BX3">
+        <v>1.944444444444444</v>
+      </c>
+      <c r="BY3">
+        <v>1.702702702702703</v>
+      </c>
+      <c r="BZ3">
+        <v>0.9090909090909094</v>
+      </c>
+      <c r="CB3">
+        <v>1</v>
+      </c>
+      <c r="CC3">
+        <v>0.8757062146892659</v>
+      </c>
+      <c r="CD3">
+        <v>8.5</v>
+      </c>
+      <c r="CE3">
+        <v>1.585365853658536</v>
+      </c>
+      <c r="CF3">
+        <v>33.40000000000001</v>
+      </c>
+      <c r="CG3">
+        <v>1.375</v>
+      </c>
+      <c r="CH3">
+        <v>1.271844660194175</v>
+      </c>
+      <c r="CI3">
+        <v>1</v>
+      </c>
+      <c r="CK3">
         <v>1.416666666666667</v>
       </c>
-      <c r="AB3">
-        <v>2.105263157894737</v>
-      </c>
-      <c r="AC3">
-        <v>0.8396226415094342</v>
-      </c>
-      <c r="AD3">
-        <v>1.265060240963856</v>
-      </c>
-      <c r="AE3">
-        <v>0.8965517241379307</v>
-      </c>
-      <c r="AF3">
-        <v>0.4074074074074074</v>
-      </c>
-      <c r="AG3">
-        <v>0.9638554216867471</v>
-      </c>
-      <c r="AH3">
-        <v>1.030075187969925</v>
-      </c>
-      <c r="AI3">
-        <v>1.415094339622641</v>
-      </c>
-      <c r="AJ3">
-        <v>1</v>
-      </c>
-      <c r="AL3">
-        <v>0.3653846153846154</v>
-      </c>
-      <c r="AN3">
-        <v>0.9917355371900825</v>
-      </c>
-      <c r="AO3">
-        <v>1.463768115942029</v>
-      </c>
-      <c r="AP3">
-        <v>10.14285714285715</v>
-      </c>
-      <c r="AQ3">
-        <v>0.9666666666666666</v>
-      </c>
-      <c r="AR3">
-        <v>1.050359712230217</v>
-      </c>
-      <c r="AV3">
-        <v>2.344827586206897</v>
-      </c>
-      <c r="AW3">
-        <v>0.9401709401709402</v>
-      </c>
-      <c r="AX3">
-        <v>1.134328358208955</v>
-      </c>
-      <c r="AY3">
-        <v>0.9161290322580646</v>
-      </c>
-      <c r="AZ3">
-        <v>0.9104477611940303</v>
-      </c>
-      <c r="BA3">
-        <v>1.219696969696969</v>
-      </c>
-      <c r="BB3">
-        <v>1.012738853503184</v>
-      </c>
-      <c r="BC3">
-        <v>2.111111111111111</v>
-      </c>
-      <c r="BD3">
-        <v>0.4943820224719102</v>
-      </c>
-      <c r="BE3">
-        <v>1.129032258064517</v>
-      </c>
-      <c r="BF3">
-        <v>0.9876543209876545</v>
-      </c>
-      <c r="BG3">
-        <v>164.0000000000001</v>
-      </c>
-      <c r="BH3">
-        <v>1.251851851851852</v>
-      </c>
-      <c r="BI3">
-        <v>2.147058823529412</v>
-      </c>
-      <c r="BJ3">
-        <v>0.9677419354838711</v>
-      </c>
-      <c r="BL3">
-        <v>0.9852941176470588</v>
-      </c>
-      <c r="BM3">
-        <v>0.6153846153846153</v>
-      </c>
-      <c r="BQ3">
-        <v>2.72549019607843</v>
-      </c>
-      <c r="BR3">
-        <v>2.108108108108108</v>
-      </c>
-      <c r="BS3">
-        <v>8.444444444444443</v>
-      </c>
-      <c r="BT3">
-        <v>0.7164179104477613</v>
-      </c>
-      <c r="BU3">
-        <v>0</v>
-      </c>
-      <c r="BV3">
-        <v>1.71875</v>
-      </c>
-      <c r="BW3">
-        <v>0.71875</v>
-      </c>
-      <c r="BX3">
-        <v>0.9881656804733731</v>
-      </c>
-      <c r="CA3">
-        <v>0.6818181818181817</v>
-      </c>
-      <c r="CB3">
-        <v>2.152777777777778</v>
-      </c>
-      <c r="CD3">
-        <v>16.44444444444444</v>
-      </c>
-      <c r="CE3">
-        <v>0.9545454545454551</v>
-      </c>
-      <c r="CF3">
-        <v>1.064935064935065</v>
-      </c>
-      <c r="CH3">
-        <v>1.478260869565218</v>
-      </c>
-      <c r="CK3">
-        <v>0.9047619047619044</v>
+      <c r="CL3">
+        <v>2.283333333333333</v>
       </c>
       <c r="CM3">
-        <v>1.025862068965518</v>
+        <v>0.9322033898305084</v>
       </c>
       <c r="CN3">
-        <v>1.271844660194175</v>
+        <v>0.5303030303030302</v>
+      </c>
+      <c r="CO3">
+        <v>1.203389830508474</v>
       </c>
       <c r="CP3">
-        <v>1.066037735849057</v>
+        <v>0.8728813559322031</v>
+      </c>
+      <c r="CQ3">
+        <v>0.9757575757575755</v>
+      </c>
+      <c r="CR3">
+        <v>1.233333333333333</v>
       </c>
       <c r="CS3">
-        <v>1.138461538461538</v>
+        <v>1</v>
+      </c>
+      <c r="CT3">
+        <v>1.375</v>
+      </c>
+      <c r="CU3">
+        <v>1.260869565217392</v>
+      </c>
+      <c r="CV3">
+        <v>1</v>
+      </c>
+      <c r="CW3">
+        <v>1.071428571428571</v>
       </c>
     </row>
     <row r="4" spans="1:101">
       <c r="A4" s="1">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>1.228571428571427</v>
+      </c>
       <c r="C4">
+        <v>2.870370370370371</v>
+      </c>
+      <c r="D4">
+        <v>1.818181818181818</v>
+      </c>
+      <c r="E4">
+        <v>1.179245283018868</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>2.911111111111111</v>
+      </c>
+      <c r="I4">
+        <v>1.388888888888889</v>
+      </c>
+      <c r="J4">
         <v>0.5638297872340425</v>
       </c>
-      <c r="D4">
-        <v>0.9761904761904762</v>
-      </c>
-      <c r="E4">
-        <v>1.126760563380282</v>
-      </c>
-      <c r="F4">
+      <c r="K4">
         <v>1.328358208955224</v>
       </c>
-      <c r="H4">
+      <c r="L4">
+        <v>3.090909090909092</v>
+      </c>
+      <c r="M4">
+        <v>1.449275362318841</v>
+      </c>
+      <c r="N4">
         <v>1.321739130434782</v>
       </c>
-      <c r="I4">
+      <c r="O4">
         <v>0.9090909090909091</v>
       </c>
-      <c r="L4">
-        <v>1.23943661971831</v>
-      </c>
-      <c r="N4">
+      <c r="P4">
+        <v>3.081632653061224</v>
+      </c>
+      <c r="Q4">
         <v>0.8641975308641975</v>
       </c>
-      <c r="Q4">
-        <v>1.878787878787879</v>
-      </c>
-      <c r="R4">
-        <v>1.378787878787879</v>
-      </c>
-      <c r="S4">
-        <v>1.220183486238532</v>
-      </c>
       <c r="T4">
-        <v>2.3</v>
+        <v>0.9371069182389938</v>
       </c>
       <c r="U4">
+        <v>0.9875776397515531</v>
+      </c>
+      <c r="V4">
+        <v>1.647058823529411</v>
+      </c>
+      <c r="W4">
+        <v>0.9390243902439024</v>
+      </c>
+      <c r="Z4">
+        <v>1.397260273972602</v>
+      </c>
+      <c r="AA4">
+        <v>0.5986842105263158</v>
+      </c>
+      <c r="AC4">
+        <v>0.8136645962732921</v>
+      </c>
+      <c r="AD4">
+        <v>1.144144144144144</v>
+      </c>
+      <c r="AF4">
+        <v>0.8689655172413789</v>
+      </c>
+      <c r="AG4">
+        <v>0.4428571428571429</v>
+      </c>
+      <c r="AI4">
+        <v>2.363636363636363</v>
+      </c>
+      <c r="AJ4">
+        <v>1.630434782608696</v>
+      </c>
+      <c r="AK4">
+        <v>1.096385542168675</v>
+      </c>
+      <c r="AL4">
+        <v>0.9652777777777775</v>
+      </c>
+      <c r="AM4">
+        <v>1.163265306122449</v>
+      </c>
+      <c r="AN4">
+        <v>0.9029850746268659</v>
+      </c>
+      <c r="AO4">
+        <v>1.121739130434782</v>
+      </c>
+      <c r="AP4">
+        <v>0.9470198675496694</v>
+      </c>
+      <c r="AQ4">
+        <v>1.647887323943662</v>
+      </c>
+      <c r="AR4">
+        <v>1.782051282051281</v>
+      </c>
+      <c r="AS4">
         <v>0</v>
       </c>
-      <c r="V4">
-        <v>2.729166666666667</v>
-      </c>
-      <c r="W4">
-        <v>1.314285714285714</v>
-      </c>
-      <c r="X4">
-        <v>2.911111111111111</v>
-      </c>
-      <c r="Y4">
-        <v>1.500000000000001</v>
-      </c>
-      <c r="AC4">
-        <v>1.377358490566038</v>
-      </c>
-      <c r="AE4">
-        <v>0.9241379310344825</v>
-      </c>
-      <c r="AF4">
-        <v>1.685185185185185</v>
-      </c>
-      <c r="AH4">
-        <v>1.075187969924813</v>
-      </c>
-      <c r="AI4">
-        <v>1.452830188679245</v>
-      </c>
-      <c r="AJ4">
-        <v>1.007462686567165</v>
-      </c>
-      <c r="AL4">
-        <v>0.09615384615384616</v>
-      </c>
-      <c r="AM4">
-        <v>0</v>
-      </c>
-      <c r="AO4">
-        <v>1.695652173913043</v>
-      </c>
-      <c r="AP4">
-        <v>10.07142857142857</v>
-      </c>
-      <c r="AQ4">
-        <v>0.9666666666666666</v>
-      </c>
-      <c r="AR4">
-        <v>0.7913669064748206</v>
-      </c>
-      <c r="AS4">
-        <v>1.07563025210084</v>
+      <c r="AT4">
+        <v>1.169642857142857</v>
+      </c>
+      <c r="AU4">
+        <v>9.687499999999998</v>
       </c>
       <c r="AV4">
-        <v>2.206896551724138</v>
+        <v>1.638888888888889</v>
       </c>
       <c r="AW4">
-        <v>0.9658119658119656</v>
+        <v>1.096774193548387</v>
       </c>
       <c r="AX4">
-        <v>1.522388059701492</v>
+        <v>4.205882352941178</v>
+      </c>
+      <c r="AY4">
+        <v>0.7799999999999998</v>
       </c>
       <c r="AZ4">
-        <v>0.761194029850746</v>
+        <v>0.9523809523809524</v>
       </c>
       <c r="BA4">
+        <v>0.3313253012048192</v>
+      </c>
+      <c r="BB4">
+        <v>1.357142857142857</v>
+      </c>
+      <c r="BC4">
+        <v>0.8115942028985511</v>
+      </c>
+      <c r="BD4">
+        <v>1.625</v>
+      </c>
+      <c r="BE4">
+        <v>0.7281553398058254</v>
+      </c>
+      <c r="BF4">
+        <v>1.764705882352941</v>
+      </c>
+      <c r="BH4">
+        <v>0.4943820224719102</v>
+      </c>
+      <c r="BI4">
+        <v>0.6141732283464567</v>
+      </c>
+      <c r="BJ4">
+        <v>0.9117647058823528</v>
+      </c>
+      <c r="BL4">
+        <v>1.388888888888889</v>
+      </c>
+      <c r="BM4">
+        <v>0.8536585365853653</v>
+      </c>
+      <c r="BN4">
+        <v>1.138888888888889</v>
+      </c>
+      <c r="BO4">
+        <v>0.8695652173913043</v>
+      </c>
+      <c r="BP4">
+        <v>48.50000000000001</v>
+      </c>
+      <c r="BQ4">
+        <v>0.8392857142857142</v>
+      </c>
+      <c r="BR4">
+        <v>1.012048192771084</v>
+      </c>
+      <c r="BS4">
+        <v>6.499999999999999</v>
+      </c>
+      <c r="BT4">
+        <v>1.2</v>
+      </c>
+      <c r="BU4">
+        <v>0.9349112426035501</v>
+      </c>
+      <c r="BV4">
+        <v>1.351351351351351</v>
+      </c>
+      <c r="BW4">
+        <v>1.0375</v>
+      </c>
+      <c r="BX4">
+        <v>1.638888888888889</v>
+      </c>
+      <c r="BY4">
+        <v>1.945945945945946</v>
+      </c>
+      <c r="BZ4">
+        <v>0.393939393939394</v>
+      </c>
+      <c r="CB4">
+        <v>1.333333333333333</v>
+      </c>
+      <c r="CC4">
+        <v>0.8700564971751413</v>
+      </c>
+      <c r="CD4">
+        <v>2.05</v>
+      </c>
+      <c r="CE4">
+        <v>1.463414634146341</v>
+      </c>
+      <c r="CF4">
+        <v>33.40000000000001</v>
+      </c>
+      <c r="CG4">
+        <v>1.625</v>
+      </c>
+      <c r="CH4">
+        <v>1.242718446601942</v>
+      </c>
+      <c r="CI4">
+        <v>172</v>
+      </c>
+      <c r="CK4">
+        <v>1.25</v>
+      </c>
+      <c r="CL4">
+        <v>1.366666666666667</v>
+      </c>
+      <c r="CM4">
+        <v>0.9152542372881356</v>
+      </c>
+      <c r="CN4">
         <v>0.5833333333333331</v>
       </c>
-      <c r="BB4">
-        <v>0.9490445859872609</v>
-      </c>
-      <c r="BC4">
-        <v>2.888888888888889</v>
-      </c>
-      <c r="BD4">
-        <v>0.50561797752809</v>
-      </c>
-      <c r="BE4">
-        <v>1.043010752688172</v>
-      </c>
-      <c r="BF4">
-        <v>0.9382716049382717</v>
-      </c>
-      <c r="BG4">
-        <v>144</v>
-      </c>
-      <c r="BH4">
-        <v>1.125925925925926</v>
-      </c>
-      <c r="BI4">
-        <v>1.308823529411764</v>
-      </c>
-      <c r="BJ4">
-        <v>0.989247311827957</v>
-      </c>
-      <c r="BL4">
-        <v>1.147058823529412</v>
-      </c>
-      <c r="BM4">
-        <v>1.076923076923077</v>
-      </c>
-      <c r="BN4">
-        <v>2.394736842105264</v>
-      </c>
-      <c r="BO4">
-        <v>1.092105263157895</v>
-      </c>
-      <c r="BR4">
-        <v>1.810810810810811</v>
-      </c>
-      <c r="BS4">
-        <v>8.111111111111111</v>
-      </c>
-      <c r="BU4">
-        <v>6.370370370370371</v>
-      </c>
-      <c r="BX4">
-        <v>0.9467455621301777</v>
-      </c>
-      <c r="BY4">
-        <v>0.3854166666666667</v>
-      </c>
-      <c r="CA4">
-        <v>1.681818181818182</v>
-      </c>
-      <c r="CE4">
-        <v>0.5909090909090908</v>
-      </c>
-      <c r="CF4">
-        <v>1</v>
-      </c>
-      <c r="CH4">
-        <v>2.173913043478261</v>
-      </c>
-      <c r="CI4">
-        <v>92</v>
-      </c>
-      <c r="CK4">
-        <v>0.952380952380952</v>
-      </c>
-      <c r="CL4">
-        <v>0.5481481481481481</v>
-      </c>
-      <c r="CM4">
-        <v>1.112068965517241</v>
-      </c>
-      <c r="CN4">
-        <v>1.242718446601942</v>
+      <c r="CO4">
+        <v>0.9576271186440674</v>
       </c>
       <c r="CP4">
-        <v>0.8207547169811322</v>
+        <v>0.9152542372881357</v>
+      </c>
+      <c r="CQ4">
+        <v>1.072727272727272</v>
+      </c>
+      <c r="CR4">
+        <v>1.083333333333333</v>
       </c>
       <c r="CS4">
-        <v>1</v>
+        <v>1.095890410958904</v>
+      </c>
+      <c r="CT4">
+        <v>1.166666666666667</v>
       </c>
       <c r="CU4">
-        <v>0.9928057553956839</v>
+        <v>2.652173913043478</v>
+      </c>
+      <c r="CV4">
+        <v>1</v>
+      </c>
+      <c r="CW4">
+        <v>0.3928571428571426</v>
       </c>
     </row>
     <row r="5" spans="1:101">
@@ -1396,193 +1510,262 @@
         <v>3</v>
       </c>
       <c r="B5">
+        <v>1.352380952380952</v>
+      </c>
+      <c r="C5">
+        <v>2.851851851851851</v>
+      </c>
+      <c r="D5">
+        <v>1.836363636363637</v>
+      </c>
+      <c r="E5">
         <v>1.443396226415095</v>
       </c>
-      <c r="C5">
+      <c r="H5">
+        <v>2.888888888888888</v>
+      </c>
+      <c r="I5">
+        <v>1.36111111111111</v>
+      </c>
+      <c r="J5">
         <v>1.202127659574468</v>
       </c>
-      <c r="D5">
-        <v>1.05952380952381</v>
-      </c>
-      <c r="F5">
+      <c r="K5">
         <v>1.462686567164179</v>
       </c>
-      <c r="G5">
-        <v>1.576470588235294</v>
-      </c>
-      <c r="H5">
+      <c r="L5">
+        <v>3.295454545454546</v>
+      </c>
+      <c r="M5">
+        <v>1.797101449275362</v>
+      </c>
+      <c r="N5">
         <v>1.182608695652174</v>
       </c>
-      <c r="I5">
+      <c r="O5">
         <v>0.9805194805194806</v>
       </c>
-      <c r="K5">
+      <c r="P5">
+        <v>3.244897959183674</v>
+      </c>
+      <c r="Q5">
+        <v>0.8271604938271605</v>
+      </c>
+      <c r="R5">
+        <v>1.307017543859649</v>
+      </c>
+      <c r="S5">
         <v>0</v>
       </c>
-      <c r="N5">
-        <v>0.8271604938271605</v>
-      </c>
-      <c r="O5">
-        <v>1.307017543859649</v>
-      </c>
-      <c r="S5">
-        <v>1.311926605504588</v>
-      </c>
-      <c r="T5">
-        <v>2.633333333333333</v>
+      <c r="U5">
+        <v>1.105590062111801</v>
       </c>
       <c r="V5">
-        <v>1.708333333333333</v>
+        <v>1.764705882352942</v>
       </c>
       <c r="W5">
-        <v>1.342857142857142</v>
-      </c>
-      <c r="X5">
-        <v>2.888888888888888</v>
-      </c>
-      <c r="Y5">
-        <v>1.871428571428571</v>
+        <v>1.024390243902439</v>
       </c>
       <c r="Z5">
-        <v>1.36111111111111</v>
-      </c>
-      <c r="AB5">
-        <v>2.403508771929824</v>
+        <v>1.876712328767123</v>
+      </c>
+      <c r="AA5">
+        <v>0.1578947368421052</v>
       </c>
       <c r="AC5">
-        <v>1.377358490566038</v>
-      </c>
-      <c r="AD5">
-        <v>1.63855421686747</v>
-      </c>
-      <c r="AE5">
-        <v>0.972413793103448</v>
-      </c>
-      <c r="AH5">
-        <v>1.165413533834587</v>
+        <v>0.9627329192546586</v>
+      </c>
+      <c r="AF5">
+        <v>0.9034482758620688</v>
+      </c>
+      <c r="AG5">
+        <v>0.6928571428571432</v>
       </c>
       <c r="AI5">
-        <v>1.226415094339622</v>
+        <v>1.181818181818182</v>
       </c>
       <c r="AJ5">
-        <v>1.059701492537314</v>
+        <v>1.282608695652174</v>
+      </c>
+      <c r="AK5">
+        <v>0.8554216867469879</v>
       </c>
       <c r="AL5">
-        <v>0.2307692307692307</v>
-      </c>
-      <c r="AO5">
-        <v>1.246376811594203</v>
+        <v>1.041666666666667</v>
+      </c>
+      <c r="AM5">
+        <v>0.9591836734693878</v>
+      </c>
+      <c r="AN5">
+        <v>1.119402985074627</v>
       </c>
       <c r="AP5">
-        <v>10.28571428571429</v>
+        <v>0.9867549668874176</v>
       </c>
       <c r="AQ5">
-        <v>1.033333333333333</v>
+        <v>1.887323943661972</v>
       </c>
       <c r="AR5">
-        <v>1.035971223021583</v>
+        <v>1.67948717948718</v>
+      </c>
+      <c r="AT5">
+        <v>1.258928571428571</v>
+      </c>
+      <c r="AU5">
+        <v>10.125</v>
       </c>
       <c r="AV5">
-        <v>2.362068965517241</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="AW5">
-        <v>1.017094017094018</v>
+        <v>0.8870967741935484</v>
       </c>
       <c r="AX5">
-        <v>1.283582089552239</v>
+        <v>4.382352941176471</v>
       </c>
       <c r="AY5">
-        <v>0.9677419354838712</v>
+        <v>0.7466666666666667</v>
       </c>
       <c r="AZ5">
-        <v>1.044776119402985</v>
+        <v>2.507936507936507</v>
       </c>
       <c r="BA5">
-        <v>1.25</v>
+        <v>0.283132530120482</v>
       </c>
       <c r="BB5">
-        <v>0.9808917197452223</v>
+        <v>1.442857142857143</v>
       </c>
       <c r="BC5">
-        <v>3.083333333333333</v>
+        <v>0.8985507246376812</v>
       </c>
       <c r="BD5">
-        <v>0.6573033707865169</v>
+        <v>0.21875</v>
       </c>
       <c r="BE5">
-        <v>0.9784946236559141</v>
+        <v>0.6116504854368933</v>
       </c>
       <c r="BF5">
-        <v>0.9691358024691362</v>
+        <v>1.955882352941176</v>
+      </c>
+      <c r="BG5">
+        <v>3.125000000000001</v>
       </c>
       <c r="BH5">
-        <v>1.177777777777778</v>
+        <v>0.5337078651685394</v>
       </c>
       <c r="BI5">
-        <v>2.058823529411764</v>
+        <v>1.15748031496063</v>
       </c>
       <c r="BJ5">
-        <v>1.204301075268818</v>
+        <v>0.5</v>
       </c>
       <c r="BL5">
-        <v>1.235294117647059</v>
+        <v>0.4166666666666665</v>
+      </c>
+      <c r="BM5">
+        <v>0.9085365853658535</v>
+      </c>
+      <c r="BN5">
+        <v>1.208333333333333</v>
+      </c>
+      <c r="BO5">
+        <v>0.9420289855072462</v>
       </c>
       <c r="BP5">
-        <v>1.199999999999999</v>
+        <v>64.99999999999999</v>
+      </c>
+      <c r="BQ5">
+        <v>0.9166666666666665</v>
       </c>
       <c r="BR5">
-        <v>4.378378378378378</v>
+        <v>0.9518072289156626</v>
       </c>
       <c r="BS5">
-        <v>8.166666666666663</v>
+        <v>6.576923076923074</v>
+      </c>
+      <c r="BT5">
+        <v>1.292307692307692</v>
       </c>
       <c r="BU5">
-        <v>6.444444444444447</v>
+        <v>0.9763313609467456</v>
       </c>
       <c r="BV5">
-        <v>1.71875</v>
+        <v>1.932432432432433</v>
+      </c>
+      <c r="BW5">
+        <v>1.1</v>
       </c>
       <c r="BX5">
-        <v>0.9644970414201185</v>
+        <v>4.805555555555554</v>
       </c>
       <c r="BY5">
-        <v>0.4479166666666666</v>
-      </c>
-      <c r="CA5">
-        <v>0.5</v>
+        <v>3.756756756756754</v>
+      </c>
+      <c r="BZ5">
+        <v>0.915151515151515</v>
+      </c>
+      <c r="CB5">
+        <v>0.1428571428571428</v>
       </c>
       <c r="CC5">
-        <v>0.925</v>
+        <v>0.8870056497175148</v>
       </c>
       <c r="CD5">
-        <v>16.11111111111111</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="CE5">
-        <v>0.3636363636363637</v>
+        <v>1.585365853658536</v>
+      </c>
+      <c r="CF5">
+        <v>34.19999999999999</v>
+      </c>
+      <c r="CG5">
+        <v>0.96875</v>
       </c>
       <c r="CH5">
-        <v>0.8260869565217392</v>
+        <v>1.398058252427185</v>
+      </c>
+      <c r="CI5">
+        <v>158</v>
       </c>
       <c r="CK5">
-        <v>0.1428571428571428</v>
+        <v>1.464285714285714</v>
+      </c>
+      <c r="CL5">
+        <v>2.466666666666666</v>
       </c>
       <c r="CM5">
-        <v>1.060344827586207</v>
+        <v>2.677966101694915</v>
       </c>
       <c r="CN5">
-        <v>1.359223300970874</v>
+        <v>1.121212121212121</v>
+      </c>
+      <c r="CO5">
+        <v>1.033898305084746</v>
       </c>
       <c r="CP5">
-        <v>1.216981132075471</v>
+        <v>1.194915254237288</v>
+      </c>
+      <c r="CQ5">
+        <v>1.024242424242424</v>
+      </c>
+      <c r="CR5">
+        <v>2.399999999999999</v>
       </c>
       <c r="CS5">
-        <v>2.076923076923077</v>
+        <v>1.958904109589042</v>
+      </c>
+      <c r="CT5">
+        <v>1.302083333333333</v>
       </c>
       <c r="CU5">
-        <v>1.071942446043166</v>
+        <v>0.4782608695652174</v>
+      </c>
+      <c r="CV5">
+        <v>1.041095890410959</v>
       </c>
       <c r="CW5">
-        <v>1.830985915492958</v>
+        <v>0.4464285714285713</v>
       </c>
     </row>
     <row r="6" spans="1:101">
@@ -1590,405 +1773,546 @@
         <v>4</v>
       </c>
       <c r="B6">
+        <v>1.38095238095238</v>
+      </c>
+      <c r="D6">
+        <v>1.2</v>
+      </c>
+      <c r="E6">
         <v>1.424528301886792</v>
       </c>
-      <c r="C6">
+      <c r="F6">
+        <v>2.538461538461539</v>
+      </c>
+      <c r="H6">
+        <v>2.955555555555555</v>
+      </c>
+      <c r="I6">
+        <v>1.425925925925925</v>
+      </c>
+      <c r="J6">
         <v>0.6276595744680851</v>
       </c>
-      <c r="D6">
-        <v>1.023809523809524</v>
-      </c>
-      <c r="F6">
+      <c r="K6">
         <v>1.328358208955224</v>
       </c>
-      <c r="G6">
-        <v>1.447058823529412</v>
-      </c>
-      <c r="H6">
+      <c r="L6">
+        <v>3.250000000000001</v>
+      </c>
+      <c r="M6">
+        <v>1.768115942028986</v>
+      </c>
+      <c r="N6">
         <v>0.8782608695652173</v>
       </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
         <v>3.387755102040817</v>
       </c>
-      <c r="M6">
-        <v>2.538461538461539</v>
-      </c>
-      <c r="N6">
+      <c r="Q6">
         <v>0.7654320987654321</v>
       </c>
-      <c r="Q6">
-        <v>1.818181818181818</v>
-      </c>
-      <c r="S6">
-        <v>1.366972477064221</v>
-      </c>
-      <c r="T6">
-        <v>2.316666666666666</v>
+      <c r="V6">
+        <v>1.458823529411765</v>
       </c>
       <c r="W6">
-        <v>1.361904761904762</v>
-      </c>
-      <c r="X6">
-        <v>2.955555555555555</v>
+        <v>0.7682926829268292</v>
       </c>
       <c r="Y6">
-        <v>1.142857142857143</v>
+        <v>1.842857142857142</v>
+      </c>
+      <c r="Z6">
+        <v>0.7945205479452055</v>
       </c>
       <c r="AA6">
-        <v>0.9383561643835613</v>
-      </c>
-      <c r="AB6">
-        <v>2.280701754385964</v>
+        <v>0.4605263157894736</v>
       </c>
       <c r="AC6">
-        <v>1.19811320754717</v>
+        <v>0.8260869565217391</v>
       </c>
       <c r="AD6">
-        <v>1.277108433734939</v>
+        <v>1.153153153153153</v>
       </c>
       <c r="AE6">
-        <v>0.8206896551724141</v>
+        <v>0.9797297297297299</v>
+      </c>
+      <c r="AF6">
+        <v>0.8413793103448277</v>
       </c>
       <c r="AG6">
-        <v>0.9698795180722889</v>
+        <v>0.6500000000000002</v>
       </c>
       <c r="AH6">
-        <v>1.165413533834587</v>
+        <v>0.9927536231884057</v>
+      </c>
+      <c r="AI6">
+        <v>1.363636363636364</v>
       </c>
       <c r="AJ6">
-        <v>0.9104477611940303</v>
+        <v>1.478260869565218</v>
       </c>
       <c r="AK6">
-        <v>0.8967741935483865</v>
+        <v>0.8433734939759036</v>
+      </c>
+      <c r="AL6">
+        <v>0.9375000000000003</v>
       </c>
       <c r="AM6">
-        <v>0.8838709677419353</v>
+        <v>1.408163265306122</v>
       </c>
       <c r="AN6">
-        <v>1.008264462809918</v>
+        <v>0.5671641791044776</v>
       </c>
       <c r="AO6">
-        <v>1.507246376811594</v>
+        <v>1.043478260869565</v>
       </c>
       <c r="AP6">
-        <v>9.928571428571425</v>
+        <v>1.019867549668874</v>
       </c>
       <c r="AQ6">
-        <v>0.9733333333333333</v>
+        <v>1.507042253521127</v>
       </c>
       <c r="AR6">
-        <v>0.4604316546762592</v>
+        <v>1.615384615384615</v>
+      </c>
+      <c r="AS6">
+        <v>1.999999999999999</v>
+      </c>
+      <c r="AT6">
+        <v>1.116071428571428</v>
+      </c>
+      <c r="AU6">
+        <v>9.687499999999998</v>
       </c>
       <c r="AV6">
-        <v>2.137931034482758</v>
+        <v>1.25</v>
       </c>
       <c r="AW6">
-        <v>0.7692307692307693</v>
+        <v>0.8548387096774192</v>
       </c>
       <c r="AX6">
-        <v>1.26865671641791</v>
+        <v>1.852941176470588</v>
+      </c>
+      <c r="AY6">
+        <v>0.7266666666666662</v>
+      </c>
+      <c r="AZ6">
+        <v>0.9841269841269841</v>
       </c>
       <c r="BA6">
-        <v>1.106060606060606</v>
+        <v>1.006024096385542</v>
       </c>
       <c r="BB6">
-        <v>0.9299363057324839</v>
+        <v>1.285714285714286</v>
+      </c>
+      <c r="BC6">
+        <v>0.7608695652173917</v>
       </c>
       <c r="BD6">
-        <v>0.5393258426966293</v>
+        <v>2.4375</v>
       </c>
       <c r="BE6">
-        <v>0.924731182795699</v>
+        <v>1.388349514563108</v>
       </c>
       <c r="BF6">
-        <v>0.9135802469135801</v>
+        <v>1.441176470588235</v>
       </c>
       <c r="BG6">
-        <v>143</v>
+        <v>1.4375</v>
+      </c>
+      <c r="BH6">
+        <v>0.4943820224719102</v>
       </c>
       <c r="BI6">
-        <v>1.191176470588235</v>
+        <v>0.5511811023622047</v>
       </c>
       <c r="BJ6">
-        <v>0.989247311827957</v>
+        <v>5.176470588235293</v>
       </c>
       <c r="BL6">
-        <v>1.058823529411764</v>
+        <v>0.5</v>
+      </c>
+      <c r="BM6">
+        <v>0.8292682926829268</v>
+      </c>
+      <c r="BN6">
+        <v>1.125</v>
       </c>
       <c r="BO6">
-        <v>1.026315789473684</v>
+        <v>0.7826086956521743</v>
+      </c>
+      <c r="BP6">
+        <v>55</v>
+      </c>
+      <c r="BQ6">
+        <v>0.8809523809523809</v>
       </c>
       <c r="BR6">
-        <v>1.648648648648649</v>
+        <v>0.9156626506024095</v>
       </c>
       <c r="BS6">
-        <v>7.555555555555556</v>
+        <v>6.307692307692309</v>
+      </c>
+      <c r="BT6">
+        <v>1.184615384615384</v>
       </c>
       <c r="BU6">
-        <v>6.185185185185189</v>
+        <v>0.9112426035502956</v>
       </c>
       <c r="BV6">
-        <v>1.9375</v>
+        <v>1.324324324324324</v>
+      </c>
+      <c r="BW6">
+        <v>0.975</v>
       </c>
       <c r="BX6">
-        <v>0.9763313609467456</v>
+        <v>4.694444444444444</v>
       </c>
       <c r="BY6">
-        <v>0.3645833333333333</v>
+        <v>1.27027027027027</v>
+      </c>
+      <c r="BZ6">
+        <v>0.7939393939393939</v>
       </c>
       <c r="CA6">
+        <v>0.8275862068965516</v>
+      </c>
+      <c r="CB6">
+        <v>0.6666666666666662</v>
+      </c>
+      <c r="CC6">
+        <v>0.9435028248587577</v>
+      </c>
+      <c r="CD6">
+        <v>8.5</v>
+      </c>
+      <c r="CE6">
+        <v>1.5</v>
+      </c>
+      <c r="CF6">
+        <v>34.80000000000001</v>
+      </c>
+      <c r="CG6">
         <v>0</v>
       </c>
-      <c r="CC6">
-        <v>1.075</v>
-      </c>
-      <c r="CD6">
-        <v>14.77777777777777</v>
-      </c>
-      <c r="CE6">
-        <v>0.8636363636363639</v>
-      </c>
-      <c r="CF6">
-        <v>1.311688311688312</v>
-      </c>
       <c r="CH6">
-        <v>1.260869565217392</v>
+        <v>1.203883495145631</v>
       </c>
       <c r="CI6">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="CJ6">
-        <v>0.8583333333333333</v>
+        <v>0.04545454545454546</v>
       </c>
       <c r="CK6">
-        <v>0.857142857142857</v>
+        <v>1.214285714285714</v>
       </c>
       <c r="CL6">
-        <v>0.8444444444444443</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="CM6">
-        <v>1.189655172413793</v>
+        <v>0.2033898305084746</v>
       </c>
       <c r="CN6">
-        <v>1.203883495145631</v>
+        <v>1.03030303030303</v>
+      </c>
+      <c r="CO6">
+        <v>0.9322033898305082</v>
       </c>
       <c r="CP6">
-        <v>1.245283018867925</v>
+        <v>1.11864406779661</v>
       </c>
       <c r="CQ6">
-        <v>6.954545454545457</v>
+        <v>1.018181818181818</v>
+      </c>
+      <c r="CR6">
+        <v>1.166666666666667</v>
       </c>
       <c r="CS6">
-        <v>0.4461538461538462</v>
+        <v>1.123287671232877</v>
       </c>
       <c r="CT6">
-        <v>0.8083333333333336</v>
+        <v>1.135416666666666</v>
+      </c>
+      <c r="CU6">
+        <v>1.913043478260869</v>
+      </c>
+      <c r="CV6">
+        <v>1.013698630136986</v>
+      </c>
+      <c r="CW6">
+        <v>0.3660714285714284</v>
       </c>
     </row>
     <row r="7" spans="1:101">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="C7">
+        <v>2.722222222222222</v>
+      </c>
+      <c r="D7">
+        <v>2.545454545454545</v>
+      </c>
+      <c r="E7">
         <v>1.377358490566038</v>
       </c>
-      <c r="C7">
+      <c r="F7">
+        <v>2.692307692307692</v>
+      </c>
+      <c r="H7">
+        <v>2.977777777777777</v>
+      </c>
+      <c r="J7">
         <v>1.521276595744681</v>
       </c>
-      <c r="D7">
-        <v>1.05952380952381</v>
-      </c>
-      <c r="F7">
+      <c r="K7">
         <v>1.940298507462686</v>
       </c>
-      <c r="G7">
+      <c r="L7">
+        <v>3.159090909090908</v>
+      </c>
+      <c r="M7">
+        <v>1.492753623188406</v>
+      </c>
+      <c r="N7">
+        <v>1.252173913043478</v>
+      </c>
+      <c r="O7">
+        <v>0.9480519480519485</v>
+      </c>
+      <c r="P7">
+        <v>3.040816326530613</v>
+      </c>
+      <c r="Q7">
+        <v>0.9135802469135803</v>
+      </c>
+      <c r="T7">
+        <v>0.9371069182389938</v>
+      </c>
+      <c r="U7">
+        <v>1.018633540372671</v>
+      </c>
+      <c r="V7">
         <v>1.305882352941177</v>
       </c>
-      <c r="H7">
-        <v>1.252173913043478</v>
-      </c>
-      <c r="I7">
-        <v>0.9480519480519485</v>
-      </c>
-      <c r="L7">
-        <v>0.943661971830986</v>
-      </c>
-      <c r="N7">
-        <v>0.9135802469135803</v>
-      </c>
-      <c r="R7">
-        <v>1.46969696969697</v>
-      </c>
-      <c r="T7">
-        <v>2.566666666666666</v>
-      </c>
-      <c r="V7">
-        <v>2.916666666666666</v>
-      </c>
-      <c r="X7">
-        <v>2.977777777777777</v>
+      <c r="W7">
+        <v>1.036585365853658</v>
       </c>
       <c r="Y7">
-        <v>2</v>
+        <v>1.714285714285714</v>
       </c>
       <c r="Z7">
-        <v>1.407407407407407</v>
+        <v>1.863013698630138</v>
       </c>
       <c r="AA7">
-        <v>0.8972602739726024</v>
+        <v>1.078947368421053</v>
       </c>
       <c r="AC7">
-        <v>1.452830188679245</v>
-      </c>
-      <c r="AD7">
-        <v>1.36144578313253</v>
+        <v>0.9378881987577641</v>
       </c>
       <c r="AE7">
-        <v>0.8620689655172414</v>
+        <v>0.9324324324324325</v>
+      </c>
+      <c r="AF7">
+        <v>0.9310344827586208</v>
+      </c>
+      <c r="AG7">
+        <v>0.7214285714285718</v>
       </c>
       <c r="AH7">
-        <v>1.082706766917293</v>
+        <v>0.9492753623188406</v>
       </c>
       <c r="AI7">
-        <v>1</v>
+        <v>1.290909090909091</v>
       </c>
       <c r="AJ7">
-        <v>1.044776119402985</v>
+        <v>1.326086956521739</v>
       </c>
       <c r="AK7">
-        <v>0.7483870967741933</v>
+        <v>0.7831325301204819</v>
       </c>
       <c r="AL7">
-        <v>2.884615384615385</v>
+        <v>0.9097222222222223</v>
       </c>
       <c r="AM7">
-        <v>0.8193548387096773</v>
+        <v>0.8571428571428573</v>
       </c>
       <c r="AO7">
-        <v>1.159420289855073</v>
+        <v>1.139130434782608</v>
       </c>
       <c r="AP7">
-        <v>10.28571428571429</v>
+        <v>0.9735099337748344</v>
       </c>
       <c r="AQ7">
-        <v>0.9399999999999996</v>
+        <v>1.563380281690141</v>
       </c>
       <c r="AR7">
-        <v>1.064748201438849</v>
+        <v>1.743589743589744</v>
+      </c>
+      <c r="AS7">
+        <v>2.079365079365079</v>
+      </c>
+      <c r="AT7">
+        <v>1.249999999999999</v>
+      </c>
+      <c r="AU7">
+        <v>9.437499999999996</v>
       </c>
       <c r="AV7">
-        <v>2.327586206896552</v>
+        <v>4.194444444444443</v>
       </c>
       <c r="AW7">
-        <v>0.9401709401709402</v>
+        <v>0.9354838709677417</v>
       </c>
       <c r="AX7">
-        <v>0.9402985074626865</v>
+        <v>4.382352941176471</v>
+      </c>
+      <c r="AY7">
+        <v>0.7599999999999998</v>
       </c>
       <c r="AZ7">
-        <v>0.5447761194029852</v>
+        <v>0.8253968253968255</v>
       </c>
       <c r="BA7">
-        <v>0.515151515151515</v>
+        <v>0.2650602409638554</v>
       </c>
       <c r="BB7">
-        <v>1.012738853503184</v>
+        <v>1.514285714285714</v>
       </c>
       <c r="BC7">
-        <v>3.388888888888889</v>
+        <v>0.7826086956521743</v>
+      </c>
+      <c r="BD7">
+        <v>5.531249999999998</v>
       </c>
       <c r="BE7">
-        <v>0.881720430107527</v>
+        <v>0.650485436893204</v>
       </c>
       <c r="BF7">
-        <v>0.9938271604938269</v>
+        <v>1.029411764705882</v>
       </c>
       <c r="BG7">
-        <v>165</v>
+        <v>1.604166666666667</v>
+      </c>
+      <c r="BH7">
+        <v>0.03370786516853933</v>
       </c>
       <c r="BI7">
-        <v>1.029411764705882</v>
+        <v>0.5984251968503937</v>
       </c>
       <c r="BJ7">
-        <v>0.8602150537634409</v>
+        <v>0.3529411764705881</v>
       </c>
       <c r="BL7">
-        <v>1.191176470588235</v>
+        <v>1.027777777777778</v>
       </c>
       <c r="BM7">
-        <v>0.9487179487179488</v>
+        <v>0.9146341463414633</v>
+      </c>
+      <c r="BN7">
+        <v>1.097222222222222</v>
+      </c>
+      <c r="BO7">
+        <v>1</v>
+      </c>
+      <c r="BP7">
+        <v>83.50000000000003</v>
+      </c>
+      <c r="BQ7">
+        <v>0.8988095238095237</v>
       </c>
       <c r="BR7">
-        <v>1.459459459459459</v>
+        <v>0.04819277108433734</v>
       </c>
       <c r="BS7">
-        <v>7.777777777777774</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="BT7">
-        <v>0.6641791044776121</v>
+        <v>1.076923076923077</v>
       </c>
       <c r="BU7">
-        <v>0.1851851851851852</v>
+        <v>0.9940828402366862</v>
       </c>
       <c r="BV7">
-        <v>1.59375</v>
+        <v>1.121621621621622</v>
       </c>
       <c r="BW7">
-        <v>0.4374999999999999</v>
+        <v>1.05</v>
       </c>
       <c r="BX7">
-        <v>1.017751479289941</v>
-      </c>
-      <c r="CA7">
-        <v>0.9090909090909093</v>
+        <v>1.5</v>
+      </c>
+      <c r="BY7">
+        <v>3.81081081081081</v>
+      </c>
+      <c r="BZ7">
+        <v>0.8363636363636363</v>
       </c>
       <c r="CB7">
-        <v>2.138888888888888</v>
+        <v>0.7142857142857137</v>
       </c>
       <c r="CC7">
-        <v>1.15</v>
+        <v>0.8700564971751413</v>
       </c>
       <c r="CD7">
-        <v>15.66666666666666</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="CE7">
-        <v>0.6818181818181817</v>
+        <v>1.597560975609756</v>
       </c>
       <c r="CF7">
-        <v>1.103896103896104</v>
+        <v>32.4</v>
       </c>
       <c r="CG7">
-        <v>1.014084507042254</v>
+        <v>1.6875</v>
       </c>
       <c r="CH7">
-        <v>2.08695652173913</v>
-      </c>
-      <c r="CJ7">
-        <v>1</v>
+        <v>1.097087378640777</v>
+      </c>
+      <c r="CI7">
+        <v>149</v>
       </c>
       <c r="CK7">
-        <v>1.285714285714285</v>
+        <v>1.261904761904761</v>
+      </c>
+      <c r="CL7">
+        <v>2.316666666666666</v>
       </c>
       <c r="CM7">
-        <v>1.103448275862069</v>
+        <v>2.813559322033898</v>
       </c>
       <c r="CN7">
-        <v>1.097087378640777</v>
+        <v>0.4772727272727271</v>
+      </c>
+      <c r="CO7">
+        <v>1.177966101694914</v>
       </c>
       <c r="CP7">
-        <v>1.245283018867925</v>
+        <v>1.11864406779661</v>
       </c>
       <c r="CQ7">
-        <v>6.999999999999999</v>
+        <v>1.066666666666667</v>
+      </c>
+      <c r="CR7">
+        <v>1.116666666666667</v>
       </c>
       <c r="CS7">
-        <v>1.123076923076923</v>
+        <v>1.726027397260273</v>
+      </c>
+      <c r="CT7">
+        <v>1.15625</v>
+      </c>
+      <c r="CU7">
+        <v>1.608695652173913</v>
+      </c>
+      <c r="CV7">
+        <v>0.9520547945205472</v>
       </c>
       <c r="CW7">
-        <v>1.746478873239437</v>
+        <v>0.3660714285714284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>